<commit_message>
Ajout de méthode pour comparer la carte et les nombres tiré dans la nouvelle classe Operation Ajout d'une classe pour les rangées, pour correspondre au JSON
</commit_message>
<xml_diff>
--- a/cartes/Datas.xlsx
+++ b/cartes/Datas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\1. HEG\Cours\Semestre 5\5. Patterns de conception\_Support de cours\_Pratique\_Java\cartes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\Librairie\MyLotoTCK\cartes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97A0F4F-DD4E-43DD-8ECB-91D5BB9DAF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBB689D-5A16-4EE5-AD63-203F911498A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8784" yWindow="2484" windowWidth="13212" windowHeight="8880" xr2:uid="{D73E7529-354C-4014-A447-01F8DE6639C6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D73E7529-354C-4014-A447-01F8DE6639C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -706,16 +706,16 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -743,7 +743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -757,7 +757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -771,7 +771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -785,7 +785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -799,7 +799,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -813,7 +813,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -841,7 +841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -855,7 +855,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -869,7 +869,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -883,7 +883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -897,7 +897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -911,7 +911,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -925,7 +925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -939,7 +939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -953,7 +953,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -967,7 +967,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -981,7 +981,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -995,7 +995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>

</xml_diff>